<commit_message>
Mise à jour Acteurs
</commit_message>
<xml_diff>
--- a/data_individu_Moyen_Orient_Japon.xlsx
+++ b/data_individu_Moyen_Orient_Japon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AELION\Desktop\Aelion\13_SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AELION\Desktop\Aelion\13_SQL\datacinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Nom</t>
   </si>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,249 +686,199 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1">
-        <v>27078</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1">
-        <v>27078</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="1">
+        <v>30507</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="D16" s="1">
+        <v>31685</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="D17" s="1">
+        <v>31381</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <v>23668</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="1">
-        <v>30507</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1">
-        <v>31685</v>
+        <v>35471</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1">
-        <v>31381</v>
+        <v>14696</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1">
-        <v>23668</v>
+        <v>19398</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="D23" s="1">
+        <v>32958</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1">
-        <v>35471</v>
+        <v>33934</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1">
-        <v>14696</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1">
-        <v>19398</v>
+        <v>32346</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1">
-        <v>32958</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="1">
-        <v>33934</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="1">
-        <v>32346</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="1">
         <v>9189</v>
       </c>
     </row>

</xml_diff>